<commit_message>
Refactor recursive Fibonacci function to handle base cases for n = 0 and n = 1; update documentation and analysis for performance comparison of iterative and recursive methods.
</commit_message>
<xml_diff>
--- a/Practical Files/exels/Practical-1.xlsx
+++ b/Practical Files/exels/Practical-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vatsal\Desktop\Sem4\DAA\Practical Files\exels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED34C010-7903-45E0-878D-1106A7B3EDF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3E7BED-50E6-42CA-8AC3-91CA08AA09A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48" yWindow="684" windowWidth="30624" windowHeight="16548" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20424" yWindow="684" windowWidth="10236" windowHeight="16548" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Value of N</t>
   </si>
@@ -41,15 +41,25 @@
   <si>
     <t>Steps in equation method</t>
   </si>
+  <si>
+    <t>Sum Of 1 To N Numbers</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF595959"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -75,8 +85,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -128,12 +141,10 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Sum</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Of 1 To N Numbers</a:t>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Sum Of 1 To N Numbers</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -172,7 +183,7 @@
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
-        <c:grouping val="stacked"/>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -239,7 +250,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8205-4F10-A2A4-7541961D4798}"/>
+              <c16:uniqueId val="{00000000-0F3C-4BCB-B6F3-8682811587AC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -252,7 +263,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Steps in recursive method</c:v>
+                  <c:v>Steps in equation method</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -308,7 +319,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-8205-4F10-A2A4-7541961D4798}"/>
+              <c16:uniqueId val="{00000001-0F3C-4BCB-B6F3-8682811587AC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -321,7 +332,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Steps in equation method</c:v>
+                  <c:v>Steps in recursive method</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -357,19 +368,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -377,7 +388,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-8205-4F10-A2A4-7541961D4798}"/>
+              <c16:uniqueId val="{00000002-0F3C-4BCB-B6F3-8682811587AC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -391,11 +402,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1407989055"/>
-        <c:axId val="1407993631"/>
+        <c:axId val="241783584"/>
+        <c:axId val="241784000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1407989055"/>
+        <c:axId val="241783584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -437,7 +448,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1407993631"/>
+        <c:crossAx val="241784000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -445,7 +456,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1407993631"/>
+        <c:axId val="241784000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -496,7 +507,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1407989055"/>
+        <c:crossAx val="241783584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -540,7 +551,7 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
+    <c:dispBlanksAs val="gap"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1131,22 +1142,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1219200</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B92D1CE6-D579-4023-822F-6CE576D7984E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC034985-B6AD-43AA-A70C-2CA1F788C1D5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1430,10 +1441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1451,10 +1462,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1468,7 +1479,7 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1482,7 +1493,7 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1496,7 +1507,7 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1510,7 +1521,7 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1524,11 +1535,17 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>15</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>